<commit_message>
updated task used in testing
</commit_message>
<xml_diff>
--- a/conditions/schedules/train_x_first/red_square_00/bottom_left/inputTrain_1.1.xlsx
+++ b/conditions/schedules/train_x_first/red_square_00/bottom_left/inputTrain_1.1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20416"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giancarlodeiana/Desktop/g-casa_children_task/conditions/schedules/train_x_first/x_increasing_steps/top_left/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\exp-gcasa-study\Desktop\g-casa_children_task\conditions\schedules\train_x_first\red_square_00\bottom_left\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B36405B4-7CD1-C542-A640-9C8DBA25803E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2770D95C-E021-4B44-975E-D2B379906F3B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="16060" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21705" windowHeight="12825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -119,9 +119,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -159,9 +159,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -194,9 +194,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -229,9 +246,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -408,12 +442,12 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -445,7 +479,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -456,19 +490,19 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="I2">
         <v>30</v>
@@ -477,7 +511,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -509,7 +543,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -541,7 +575,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -573,7 +607,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -605,7 +639,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -637,7 +671,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -669,7 +703,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -680,19 +714,19 @@
         <v>4</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E9">
         <v>4</v>
       </c>
       <c r="F9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G9">
         <v>0</v>
       </c>
       <c r="H9">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="I9">
         <v>30</v>
@@ -701,7 +735,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -733,7 +767,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -765,7 +799,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -776,19 +810,19 @@
         <v>2</v>
       </c>
       <c r="D12">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E12">
         <v>2</v>
       </c>
       <c r="F12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G12">
         <v>0</v>
       </c>
       <c r="H12">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="I12">
         <v>30</v>
@@ -797,7 +831,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -829,7 +863,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -861,7 +895,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -893,7 +927,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -925,7 +959,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -957,7 +991,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -989,7 +1023,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1021,7 +1055,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1032,19 +1066,19 @@
         <v>3</v>
       </c>
       <c r="D20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E20">
         <v>3</v>
       </c>
       <c r="F20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G20">
         <v>0</v>
       </c>
       <c r="H20">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="I20">
         <v>30</v>
@@ -1053,7 +1087,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1085,7 +1119,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1096,19 +1130,19 @@
         <v>2</v>
       </c>
       <c r="D22">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E22">
         <v>2</v>
       </c>
       <c r="F22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G22">
         <v>0</v>
       </c>
       <c r="H22">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="I22">
         <v>30</v>
@@ -1117,7 +1151,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1149,7 +1183,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1181,7 +1215,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1213,7 +1247,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1245,7 +1279,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1277,7 +1311,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1288,19 +1322,19 @@
         <v>1</v>
       </c>
       <c r="D28">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E28">
         <v>1</v>
       </c>
       <c r="F28">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G28">
         <v>0</v>
       </c>
       <c r="H28">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="I28">
         <v>30</v>
@@ -1309,7 +1343,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1341,7 +1375,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1373,7 +1407,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>

</xml_diff>